<commit_message>
Revert "weekly training updates"
This reverts commit ca846b6b927b2e373d9d4b2b4448a7489f146c8a.
</commit_message>
<xml_diff>
--- a/Training_Timesheet/Weekly-Timesheet.xlsx
+++ b/Training_Timesheet/Weekly-Timesheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91933\Documents\github\sohum_traning\Training_Timesheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sss\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66F2440-F7C2-468C-AA72-821005B65ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Schedule" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <definedName name="Interval">'Weekly Schedule'!$H$4</definedName>
     <definedName name="ScheduleStart">'Weekly Schedule'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>SUN</t>
   </si>
@@ -99,114 +98,12 @@
   </si>
   <si>
     <t>00 MIN</t>
-  </si>
-  <si>
-    <t>learnt modals,popovers,tooltips</t>
-  </si>
-  <si>
-    <t>implemented through code</t>
-  </si>
-  <si>
-    <t>bootstrap components</t>
-  </si>
-  <si>
-    <t>wrote a sample program</t>
-  </si>
-  <si>
-    <t>scroll spy</t>
-  </si>
-  <si>
-    <t>done a sample program</t>
-  </si>
-  <si>
-    <t>app landing page project</t>
-  </si>
-  <si>
-    <t>learnt about ajax in jquery</t>
-  </si>
-  <si>
-    <t>regular expression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">done a form project </t>
-  </si>
-  <si>
-    <t>learnt jQuery UI and implementation</t>
-  </si>
-  <si>
-    <t>Done draggables, dropabbles</t>
-  </si>
-  <si>
-    <t>done resizables, accordians</t>
-  </si>
-  <si>
-    <t>learnt sortables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">done sample program </t>
-  </si>
-  <si>
-    <t>learnt about get and post method in jquery</t>
-  </si>
-  <si>
-    <t>learnt about get and post method in javascript</t>
-  </si>
-  <si>
-    <t>studied about node js</t>
-  </si>
-  <si>
-    <t>program on it</t>
-  </si>
-  <si>
-    <t>installed postman and node js</t>
-  </si>
-  <si>
-    <t>creating application</t>
-  </si>
-  <si>
-    <t>setting up web server</t>
-  </si>
-  <si>
-    <t>configuring and connecting to database</t>
-  </si>
-  <si>
-    <t>defining note models in mongoose</t>
-  </si>
-  <si>
-    <t>studied about mongodb</t>
-  </si>
-  <si>
-    <t>written sample program</t>
-  </si>
-  <si>
-    <t>studied about mongoose packages</t>
-  </si>
-  <si>
-    <t>operations in mongodb</t>
-  </si>
-  <si>
-    <t>defining routes using express</t>
-  </si>
-  <si>
-    <t>written code for it</t>
-  </si>
-  <si>
-    <t>creating a new note</t>
-  </si>
-  <si>
-    <t>retriving all notes and a single note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">updating note </t>
-  </si>
-  <si>
-    <t>CRUD operations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
@@ -882,27 +779,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="9" width="23.90625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="1.90625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.6328125" style="1"/>
+    <col min="3" max="9" width="23.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="1.88671875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34"/>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -914,7 +811,7 @@
       <c r="I1" s="34"/>
       <c r="J1" s="34"/>
     </row>
-    <row r="2" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34"/>
       <c r="B2" s="39" t="s">
         <v>21</v>
@@ -934,13 +831,13 @@
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
     </row>
-    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="40"/>
       <c r="E3" s="9">
-        <v>0.41666666666666669</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>17</v>
@@ -967,35 +864,35 @@
       <c r="I4" s="35"/>
       <c r="J4" s="34"/>
     </row>
-    <row r="5" spans="1:10" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34"/>
       <c r="B5" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="E5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="F5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="G5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="I5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>0</v>
-      </c>
       <c r="J5" s="34"/>
     </row>
-    <row r="6" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" s="38"/>
       <c r="C6" s="16">
@@ -1028,61 +925,41 @@
       </c>
       <c r="J6" s="34"/>
     </row>
-    <row r="7" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" s="20">
         <f>E3</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>49</v>
-      </c>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="23"/>
       <c r="I7" s="22"/>
       <c r="J7" s="34"/>
     </row>
-    <row r="8" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" s="21">
-        <f t="shared" ref="B8:B20" si="1">B7+TIME(0,Interval,0)</f>
-        <v>0.45833333333333337</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="28" t="s">
-        <v>50</v>
-      </c>
+        <f t="shared" ref="B8:B32" si="1">B7+TIME(0,Interval,0)</f>
+        <v>0.25</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="27"/>
       <c r="I8" s="26"/>
       <c r="J8" s="34"/>
     </row>
-    <row r="9" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" s="20">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="31"/>
@@ -1093,34 +970,26 @@
       <c r="I9" s="30"/>
       <c r="J9" s="34"/>
     </row>
-    <row r="10" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" s="21">
         <f t="shared" si="1"/>
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>32</v>
-      </c>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="28"/>
-      <c r="F10" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>51</v>
-      </c>
+      <c r="F10" s="29"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="27"/>
       <c r="I10" s="26"/>
       <c r="J10" s="34"/>
     </row>
-    <row r="11" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" s="20">
         <f t="shared" si="1"/>
-        <v>0.58333333333333326</v>
+        <v>0.37500000000000006</v>
       </c>
       <c r="C11" s="30"/>
       <c r="D11" s="31"/>
@@ -1131,11 +1000,11 @@
       <c r="I11" s="30"/>
       <c r="J11" s="34"/>
     </row>
-    <row r="12" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="34"/>
       <c r="B12" s="21">
         <f t="shared" si="1"/>
-        <v>0.62499999999999989</v>
+        <v>0.41666666666666674</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="27"/>
@@ -1146,11 +1015,11 @@
       <c r="I12" s="26"/>
       <c r="J12" s="34"/>
     </row>
-    <row r="13" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="34"/>
       <c r="B13" s="20">
         <f t="shared" si="1"/>
-        <v>0.66666666666666652</v>
+        <v>0.45833333333333343</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="31"/>
@@ -1161,11 +1030,11 @@
       <c r="I13" s="30"/>
       <c r="J13" s="34"/>
     </row>
-    <row r="14" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34"/>
       <c r="B14" s="21">
         <f t="shared" si="1"/>
-        <v>0.70833333333333315</v>
+        <v>0.50000000000000011</v>
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="27"/>
@@ -1176,93 +1045,59 @@
       <c r="I14" s="26"/>
       <c r="J14" s="34"/>
     </row>
-    <row r="15" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
       <c r="B15" s="20">
         <f t="shared" si="1"/>
-        <v>0.74999999999999978</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="32" t="s">
-        <v>56</v>
-      </c>
+        <v>0.54166666666666674</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="32"/>
       <c r="H15" s="31"/>
       <c r="I15" s="30"/>
       <c r="J15" s="34"/>
     </row>
-    <row r="16" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34"/>
       <c r="B16" s="21">
         <f t="shared" si="1"/>
-        <v>0.79166666666666641</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="28" t="s">
-        <v>52</v>
-      </c>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="28"/>
       <c r="H16" s="27"/>
       <c r="I16" s="26"/>
       <c r="J16" s="34"/>
     </row>
-    <row r="17" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34"/>
       <c r="B17" s="20">
         <f t="shared" si="1"/>
-        <v>0.83333333333333304</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="32" t="s">
-        <v>53</v>
-      </c>
+        <v>0.625</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="32"/>
       <c r="H17" s="31"/>
       <c r="I17" s="30"/>
       <c r="J17" s="34"/>
     </row>
-    <row r="18" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34"/>
       <c r="B18" s="21">
         <f t="shared" si="1"/>
-        <v>0.87499999999999967</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>35</v>
-      </c>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
       <c r="E18" s="28"/>
       <c r="F18" s="29"/>
       <c r="G18" s="28"/>
@@ -1270,47 +1105,42 @@
       <c r="I18" s="26"/>
       <c r="J18" s="34"/>
     </row>
-    <row r="19" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34"/>
       <c r="B19" s="20">
         <f t="shared" si="1"/>
-        <v>0.9166666666666663</v>
+        <v>0.70833333333333326</v>
       </c>
       <c r="C19" s="30"/>
-      <c r="D19" s="31" t="s">
-        <v>36</v>
-      </c>
+      <c r="D19" s="31"/>
       <c r="E19" s="32"/>
       <c r="F19" s="33"/>
-      <c r="G19" s="32" t="s">
-        <v>54</v>
-      </c>
+      <c r="G19" s="32"/>
       <c r="H19" s="31"/>
       <c r="I19" s="30"/>
       <c r="J19" s="34"/>
     </row>
-    <row r="20" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34"/>
       <c r="B20" s="21">
         <f t="shared" si="1"/>
-        <v>0.95833333333333293</v>
+        <v>0.74999999999999989</v>
       </c>
       <c r="C20" s="26"/>
-      <c r="D20" s="27" t="s">
-        <v>37</v>
-      </c>
+      <c r="D20" s="27"/>
       <c r="E20" s="28"/>
       <c r="F20" s="29"/>
-      <c r="G20" s="28" t="s">
-        <v>55</v>
-      </c>
+      <c r="G20" s="28"/>
       <c r="H20" s="27"/>
       <c r="I20" s="26"/>
       <c r="J20" s="34"/>
     </row>
-    <row r="21" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="34"/>
-      <c r="B21" s="20"/>
+      <c r="B21" s="20">
+        <f t="shared" si="1"/>
+        <v>0.79166666666666652</v>
+      </c>
       <c r="C21" s="30"/>
       <c r="D21" s="31"/>
       <c r="E21" s="32"/>
@@ -1320,9 +1150,12 @@
       <c r="I21" s="30"/>
       <c r="J21" s="34"/>
     </row>
-    <row r="22" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="34"/>
-      <c r="B22" s="21"/>
+      <c r="B22" s="21">
+        <f t="shared" si="1"/>
+        <v>0.83333333333333315</v>
+      </c>
       <c r="C22" s="26"/>
       <c r="D22" s="27"/>
       <c r="E22" s="28"/>
@@ -1332,9 +1165,12 @@
       <c r="I22" s="26"/>
       <c r="J22" s="34"/>
     </row>
-    <row r="23" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="34"/>
-      <c r="B23" s="20"/>
+      <c r="B23" s="20">
+        <f t="shared" si="1"/>
+        <v>0.87499999999999978</v>
+      </c>
       <c r="C23" s="30"/>
       <c r="D23" s="31"/>
       <c r="E23" s="32"/>
@@ -1344,9 +1180,12 @@
       <c r="I23" s="30"/>
       <c r="J23" s="34"/>
     </row>
-    <row r="24" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="34"/>
-      <c r="B24" s="21"/>
+      <c r="B24" s="21">
+        <f t="shared" si="1"/>
+        <v>0.91666666666666641</v>
+      </c>
       <c r="C24" s="26"/>
       <c r="D24" s="27"/>
       <c r="E24" s="28"/>
@@ -1356,9 +1195,12 @@
       <c r="I24" s="26"/>
       <c r="J24" s="34"/>
     </row>
-    <row r="25" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
-      <c r="B25" s="20"/>
+      <c r="B25" s="20">
+        <f t="shared" si="1"/>
+        <v>0.95833333333333304</v>
+      </c>
       <c r="C25" s="30"/>
       <c r="D25" s="31"/>
       <c r="E25" s="32"/>
@@ -1368,9 +1210,12 @@
       <c r="I25" s="30"/>
       <c r="J25" s="34"/>
     </row>
-    <row r="26" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="34"/>
-      <c r="B26" s="21"/>
+      <c r="B26" s="21">
+        <f t="shared" si="1"/>
+        <v>0.99999999999999967</v>
+      </c>
       <c r="C26" s="26"/>
       <c r="D26" s="27"/>
       <c r="E26" s="28"/>
@@ -1380,9 +1225,12 @@
       <c r="I26" s="26"/>
       <c r="J26" s="34"/>
     </row>
-    <row r="27" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="34"/>
-      <c r="B27" s="20"/>
+      <c r="B27" s="20">
+        <f t="shared" si="1"/>
+        <v>1.0416666666666663</v>
+      </c>
       <c r="C27" s="30"/>
       <c r="D27" s="31"/>
       <c r="E27" s="32"/>
@@ -1392,9 +1240,12 @@
       <c r="I27" s="30"/>
       <c r="J27" s="34"/>
     </row>
-    <row r="28" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="34"/>
-      <c r="B28" s="21"/>
+      <c r="B28" s="21">
+        <f t="shared" si="1"/>
+        <v>1.083333333333333</v>
+      </c>
       <c r="C28" s="26"/>
       <c r="D28" s="27"/>
       <c r="E28" s="28"/>
@@ -1404,9 +1255,12 @@
       <c r="I28" s="26"/>
       <c r="J28" s="34"/>
     </row>
-    <row r="29" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34"/>
-      <c r="B29" s="20"/>
+      <c r="B29" s="20">
+        <f t="shared" si="1"/>
+        <v>1.1249999999999998</v>
+      </c>
       <c r="C29" s="30"/>
       <c r="D29" s="31"/>
       <c r="E29" s="32"/>
@@ -1416,9 +1270,12 @@
       <c r="I29" s="30"/>
       <c r="J29" s="34"/>
     </row>
-    <row r="30" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="34"/>
-      <c r="B30" s="21"/>
+      <c r="B30" s="21">
+        <f t="shared" si="1"/>
+        <v>1.1666666666666665</v>
+      </c>
       <c r="C30" s="26"/>
       <c r="D30" s="27"/>
       <c r="E30" s="28"/>
@@ -1428,9 +1285,12 @@
       <c r="I30" s="26"/>
       <c r="J30" s="34"/>
     </row>
-    <row r="31" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="34"/>
-      <c r="B31" s="20"/>
+      <c r="B31" s="20">
+        <f t="shared" si="1"/>
+        <v>1.2083333333333333</v>
+      </c>
       <c r="C31" s="30"/>
       <c r="D31" s="31"/>
       <c r="E31" s="32"/>
@@ -1440,9 +1300,12 @@
       <c r="I31" s="30"/>
       <c r="J31" s="34"/>
     </row>
-    <row r="32" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="34"/>
-      <c r="B32" s="21"/>
+      <c r="B32" s="21">
+        <f t="shared" si="1"/>
+        <v>1.25</v>
+      </c>
       <c r="C32" s="26"/>
       <c r="D32" s="27"/>
       <c r="E32" s="28"/>
@@ -1462,13 +1325,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Data Settings'!$D$3:$D$13</xm:f>
           </x14:formula1>
           <xm:sqref>F3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Data Settings'!$B$3:$B$17</xm:f>
           </x14:formula1>
@@ -1484,7 +1347,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -1494,22 +1357,22 @@
       <selection activeCell="A18" sqref="A18:XFD29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.90625" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="3.36328125" customWidth="1"/>
-    <col min="5" max="5" width="2.453125" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" customWidth="1"/>
+    <col min="5" max="5" width="2.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="4" t="s">
         <v>8</v>
@@ -1520,7 +1383,7 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="2">
         <v>0.20833333333333334</v>
@@ -1531,7 +1394,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="2">
         <v>0.25</v>
@@ -1542,7 +1405,7 @@
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="2">
         <v>0.29166666666666669</v>
@@ -1553,7 +1416,7 @@
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="2">
         <v>0.33333333333333331</v>
@@ -1564,7 +1427,7 @@
       </c>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="2">
         <v>0.375</v>
@@ -1575,7 +1438,7 @@
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="2">
         <v>0.41666666666666669</v>
@@ -1586,7 +1449,7 @@
       </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="2">
         <v>0.45833333333333331</v>
@@ -1597,7 +1460,7 @@
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="2">
         <v>0.5</v>
@@ -1608,7 +1471,7 @@
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="2">
         <v>0.54166666666666663</v>
@@ -1619,7 +1482,7 @@
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="2">
         <v>0.58333333333333337</v>
@@ -1630,7 +1493,7 @@
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="2">
         <v>0.625</v>
@@ -1641,7 +1504,7 @@
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="2">
         <v>0.66666666666666663</v>
@@ -1650,7 +1513,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="2">
         <v>0.70833333333333337</v>
@@ -1659,7 +1522,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="2">
         <v>0.75</v>
@@ -1668,7 +1531,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="2">
         <v>0.79166666666666663</v>

</xml_diff>